<commit_message>
create data transaction GMP
</commit_message>
<xml_diff>
--- a/Rancangan Database Penjadwalan.xlsx
+++ b/Rancangan Database Penjadwalan.xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25407"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github-repository\php-project\php-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748F7C9A-DAFE-4BDB-8D6D-D07B62EA28D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
   <si>
     <t>Kelas</t>
   </si>
@@ -43,12 +59,6 @@
     <t>Kode</t>
   </si>
   <si>
-    <t xml:space="preserve">Nama </t>
-  </si>
-  <si>
-    <t>Kategori</t>
-  </si>
-  <si>
     <t>Pendidikan Agama dan Budi Pekerti (Agama Lainnya)</t>
   </si>
   <si>
@@ -419,13 +429,22 @@
   </si>
   <si>
     <t>Kode_GMP</t>
+  </si>
+  <si>
+    <t>kode_mapel</t>
+  </si>
+  <si>
+    <t>nama_mapel</t>
+  </si>
+  <si>
+    <t>kategori_ mapel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +489,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -516,7 +543,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,9 +575,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,6 +627,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -757,74 +820,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14:K21"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="4" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="8.85546875" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="44" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="17" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="14.21875" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="8.85546875" customWidth="1" outlineLevel="1"/>
     <col min="22" max="22" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="14.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="18.21875" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="11.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="13.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="8.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="35" width="8.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="8.88671875" collapsed="1"/>
-    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="18.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="11.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="13.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="8.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="35" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="8.85546875" collapsed="1"/>
+    <col min="38" max="38" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>69</v>
-      </c>
       <c r="AJ1" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AK1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -841,13 +904,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -856,37 +919,37 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>60</v>
       </c>
-      <c r="R2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>132</v>
+      </c>
+      <c r="W2" t="s">
         <v>62</v>
       </c>
-      <c r="U2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
-        <v>134</v>
-      </c>
-      <c r="W2" t="s">
-        <v>64</v>
-      </c>
       <c r="X2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z2" t="s">
         <v>1</v>
@@ -895,16 +958,16 @@
         <v>8</v>
       </c>
       <c r="AB2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AD2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AE2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AG2" t="s">
         <v>1</v>
@@ -913,25 +976,25 @@
         <v>8</v>
       </c>
       <c r="AI2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AK2" t="s">
         <v>1</v>
       </c>
       <c r="AL2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AM2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AN2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AO2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -948,36 +1011,35 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <f>I3&amp;1</f>
-        <v>AK1</v>
+      <c r="G3">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M3">
         <v>10003</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R3" t="str">
         <f>"0"&amp;88728372772</f>
@@ -995,16 +1057,16 @@
         <v>AK1g0010</v>
       </c>
       <c r="W3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="X3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AB3" s="1">
         <v>0.29166666666666669</v>
@@ -1023,17 +1085,17 @@
         <v>1</v>
       </c>
       <c r="AH3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AI3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AN3" s="1" t="str">
         <f>TEXT(AB3,"hh:mm")&amp;" - "&amp;TEXT(AC3,"hh:mm")</f>
         <v>07:00 - 07:45</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1050,37 +1112,36 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" ref="G4:G11" si="3">I4&amp;(MID(G3,3,100)+1)</f>
-        <v>AK2</v>
+      <c r="G4">
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M4">
         <f>M3+1</f>
         <v>10004</v>
       </c>
       <c r="N4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" t="s">
         <v>115</v>
       </c>
-      <c r="O4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>117</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>119</v>
       </c>
       <c r="R4" t="str">
         <f>"0"&amp;R3+1</f>
@@ -1094,21 +1155,21 @@
         <v>2</v>
       </c>
       <c r="V4" t="str">
-        <f t="shared" ref="V4:V10" si="4">X4&amp;W4</f>
-        <v>AK2g0010</v>
+        <f t="shared" ref="V4:V10" si="3">X4&amp;W4</f>
+        <v>2g0010</v>
       </c>
       <c r="W4" t="s">
-        <v>112</v>
-      </c>
-      <c r="X4" t="str">
-        <f t="shared" ref="X4:X10" si="5">G4</f>
-        <v>AK2</v>
+        <v>110</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X10" si="4">G4</f>
+        <v>2</v>
       </c>
       <c r="Z4">
         <v>2</v>
       </c>
       <c r="AA4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AB4" s="1">
         <f>AC3</f>
@@ -1128,17 +1189,17 @@
         <v>2</v>
       </c>
       <c r="AH4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AI4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AN4" s="1" t="str">
-        <f t="shared" ref="AN4:AN13" si="6">TEXT(AB4,"hh:mm")&amp;" - "&amp;TEXT(AC4,"hh:mm")</f>
+        <f t="shared" ref="AN4:AN13" si="5">TEXT(AB4,"hh:mm")&amp;" - "&amp;TEXT(AC4,"hh:mm")</f>
         <v>07:45 - 08:30</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1155,40 +1216,39 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" t="str">
-        <f t="shared" si="3"/>
-        <v>AK3</v>
+      <c r="G5">
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M12" si="7">M4+1</f>
+        <f t="shared" ref="M5:M12" si="6">M4+1</f>
         <v>10005</v>
       </c>
       <c r="N5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" ref="R5:R12" si="8">"0"&amp;R4+1</f>
+        <f t="shared" ref="R5:R12" si="7">"0"&amp;R4+1</f>
         <v>088728372774</v>
       </c>
       <c r="S5" t="str">
@@ -1199,24 +1259,24 @@
         <v>3</v>
       </c>
       <c r="V5" t="str">
+        <f t="shared" si="3"/>
+        <v>3g0010</v>
+      </c>
+      <c r="W5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X5">
         <f t="shared" si="4"/>
-        <v>AK3g0010</v>
-      </c>
-      <c r="W5" t="s">
-        <v>112</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="5"/>
-        <v>AK3</v>
+        <v>3</v>
       </c>
       <c r="Z5">
         <v>3</v>
       </c>
       <c r="AA5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AB5" s="1">
-        <f t="shared" ref="AB5:AB13" si="9">AC4</f>
+        <f t="shared" ref="AB5:AB13" si="8">AC4</f>
         <v>0.35416666666666669</v>
       </c>
       <c r="AC5" s="1">
@@ -1233,17 +1293,17 @@
         <v>3</v>
       </c>
       <c r="AH5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AI5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AN5" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>08:30 - 09:15</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1260,40 +1320,39 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="3"/>
-        <v>AK4</v>
+      <c r="G6">
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M6">
+        <f t="shared" si="6"/>
+        <v>10006</v>
+      </c>
+      <c r="N6" t="s">
+        <v>119</v>
+      </c>
+      <c r="O6" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>117</v>
+      </c>
+      <c r="R6" t="str">
         <f t="shared" si="7"/>
-        <v>10006</v>
-      </c>
-      <c r="N6" t="s">
-        <v>121</v>
-      </c>
-      <c r="O6" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>119</v>
-      </c>
-      <c r="R6" t="str">
-        <f t="shared" si="8"/>
         <v>088728372775</v>
       </c>
       <c r="S6" t="str">
@@ -1304,24 +1363,24 @@
         <v>4</v>
       </c>
       <c r="V6" t="str">
+        <f t="shared" si="3"/>
+        <v>4g0010</v>
+      </c>
+      <c r="W6" t="s">
+        <v>110</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="4"/>
-        <v>AK4g0010</v>
-      </c>
-      <c r="W6" t="s">
-        <v>112</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="5"/>
-        <v>AK4</v>
+        <v>4</v>
       </c>
       <c r="Z6">
         <v>4</v>
       </c>
       <c r="AA6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AB6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.38541666666666669</v>
       </c>
       <c r="AC6" s="1">
@@ -1333,23 +1392,23 @@
         <v>0 Jam 15 Menit</v>
       </c>
       <c r="AE6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AG6">
         <v>4</v>
       </c>
       <c r="AH6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AI6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN6" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>09:15 - 09:30</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1366,40 +1425,39 @@
       <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="3"/>
-        <v>AK5</v>
+      <c r="G7">
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
       </c>
       <c r="K7">
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M7">
+        <f t="shared" si="6"/>
+        <v>10007</v>
+      </c>
+      <c r="N7" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R7" t="str">
         <f t="shared" si="7"/>
-        <v>10007</v>
-      </c>
-      <c r="N7" t="s">
-        <v>122</v>
-      </c>
-      <c r="O7" t="s">
-        <v>114</v>
-      </c>
-      <c r="P7" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>118</v>
-      </c>
-      <c r="R7" t="str">
-        <f t="shared" si="8"/>
         <v>088728372776</v>
       </c>
       <c r="S7" t="str">
@@ -1410,28 +1468,28 @@
         <v>5</v>
       </c>
       <c r="V7" t="str">
+        <f t="shared" si="3"/>
+        <v>5g0010</v>
+      </c>
+      <c r="W7" t="s">
+        <v>110</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="4"/>
-        <v>AK5g0010</v>
-      </c>
-      <c r="W7" t="s">
-        <v>112</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="5"/>
-        <v>AK5</v>
+        <v>5</v>
       </c>
       <c r="Z7">
         <v>5</v>
       </c>
       <c r="AA7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AB7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.39583333333333337</v>
       </c>
       <c r="AC7" s="1">
-        <f t="shared" ref="AC7:AC13" si="10">AB7+45/1440</f>
+        <f t="shared" ref="AC7:AC13" si="9">AB7+45/1440</f>
         <v>0.42708333333333337</v>
       </c>
       <c r="AD7" t="str">
@@ -1445,17 +1503,17 @@
         <v>5</v>
       </c>
       <c r="AH7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AI7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AN7" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>09:30 - 10:15</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1472,40 +1530,39 @@
       <c r="F8">
         <v>6</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="3"/>
-        <v>AK6</v>
+      <c r="G8">
+        <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
       </c>
       <c r="K8">
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M8">
+        <f t="shared" si="6"/>
+        <v>10008</v>
+      </c>
+      <c r="N8" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" t="s">
+        <v>112</v>
+      </c>
+      <c r="P8" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>117</v>
+      </c>
+      <c r="R8" t="str">
         <f t="shared" si="7"/>
-        <v>10008</v>
-      </c>
-      <c r="N8" t="s">
-        <v>123</v>
-      </c>
-      <c r="O8" t="s">
-        <v>114</v>
-      </c>
-      <c r="P8" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>119</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" si="8"/>
         <v>088728372777</v>
       </c>
       <c r="S8" t="str">
@@ -1516,28 +1573,28 @@
         <v>6</v>
       </c>
       <c r="V8" t="str">
+        <f t="shared" si="3"/>
+        <v>6g0010</v>
+      </c>
+      <c r="W8" t="s">
+        <v>110</v>
+      </c>
+      <c r="X8">
         <f t="shared" si="4"/>
-        <v>AK6g0010</v>
-      </c>
-      <c r="W8" t="s">
-        <v>112</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="5"/>
-        <v>AK6</v>
+        <v>6</v>
       </c>
       <c r="Z8">
         <v>6</v>
       </c>
       <c r="AA8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AB8" s="1">
+        <f t="shared" si="8"/>
+        <v>0.42708333333333337</v>
+      </c>
+      <c r="AC8" s="1">
         <f t="shared" si="9"/>
-        <v>0.42708333333333337</v>
-      </c>
-      <c r="AC8" s="1">
-        <f t="shared" si="10"/>
         <v>0.45833333333333337</v>
       </c>
       <c r="AD8" t="str">
@@ -1548,11 +1605,11 @@
         <v>5</v>
       </c>
       <c r="AN8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10:15 - 11:00</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1569,40 +1626,39 @@
       <c r="F9">
         <v>7</v>
       </c>
-      <c r="G9" t="str">
-        <f t="shared" si="3"/>
-        <v>AK7</v>
+      <c r="G9">
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
       </c>
       <c r="K9">
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M9">
+        <f t="shared" si="6"/>
+        <v>10009</v>
+      </c>
+      <c r="N9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" t="s">
+        <v>124</v>
+      </c>
+      <c r="P9" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>117</v>
+      </c>
+      <c r="R9" t="str">
         <f t="shared" si="7"/>
-        <v>10009</v>
-      </c>
-      <c r="N9" t="s">
-        <v>124</v>
-      </c>
-      <c r="O9" t="s">
-        <v>126</v>
-      </c>
-      <c r="P9" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>119</v>
-      </c>
-      <c r="R9" t="str">
-        <f t="shared" si="8"/>
         <v>088728372778</v>
       </c>
       <c r="S9" t="str">
@@ -1613,28 +1669,28 @@
         <v>7</v>
       </c>
       <c r="V9" t="str">
+        <f t="shared" si="3"/>
+        <v>7g0010</v>
+      </c>
+      <c r="W9" t="s">
+        <v>110</v>
+      </c>
+      <c r="X9">
         <f t="shared" si="4"/>
-        <v>AK7g0010</v>
-      </c>
-      <c r="W9" t="s">
-        <v>112</v>
-      </c>
-      <c r="X9" t="str">
-        <f t="shared" si="5"/>
-        <v>AK7</v>
+        <v>7</v>
       </c>
       <c r="Z9">
         <v>7</v>
       </c>
       <c r="AA9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AB9" s="1">
+        <f t="shared" si="8"/>
+        <v>0.45833333333333337</v>
+      </c>
+      <c r="AC9" s="1">
         <f t="shared" si="9"/>
-        <v>0.45833333333333337</v>
-      </c>
-      <c r="AC9" s="1">
-        <f t="shared" si="10"/>
         <v>0.48958333333333337</v>
       </c>
       <c r="AD9" t="str">
@@ -1645,11 +1701,11 @@
         <v>6</v>
       </c>
       <c r="AN9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11:00 - 11:45</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1666,68 +1722,67 @@
       <c r="F10">
         <v>8</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="3"/>
-        <v>AK8</v>
+      <c r="G10">
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
       </c>
       <c r="K10">
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M10">
+        <f t="shared" si="6"/>
+        <v>10010</v>
+      </c>
+      <c r="N10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P10" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>116</v>
+      </c>
+      <c r="R10" t="str">
         <f t="shared" si="7"/>
-        <v>10010</v>
-      </c>
-      <c r="N10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O10" t="s">
-        <v>116</v>
-      </c>
-      <c r="P10" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>118</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" si="8"/>
         <v>088728372779</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" ref="S10:S12" si="11">LOWER(SUBSTITUTE(N10," ","."))&amp;"@gmail.com"</f>
+        <f t="shared" ref="S10:S12" si="10">LOWER(SUBSTITUTE(N10," ","."))&amp;"@gmail.com"</f>
         <v>ono.jaya@gmail.com</v>
       </c>
       <c r="U10">
         <v>8</v>
       </c>
       <c r="V10" t="str">
+        <f t="shared" si="3"/>
+        <v>8g0010</v>
+      </c>
+      <c r="W10" t="s">
+        <v>110</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="4"/>
-        <v>AK8g0010</v>
-      </c>
-      <c r="W10" t="s">
-        <v>112</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="5"/>
-        <v>AK8</v>
+        <v>8</v>
       </c>
       <c r="Z10">
         <v>8</v>
       </c>
       <c r="AA10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.48958333333333337</v>
       </c>
       <c r="AC10" s="1">
@@ -1739,14 +1794,14 @@
         <v>1 Jam 0 Menit</v>
       </c>
       <c r="AE10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AN10" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11:45 - 12:45</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1763,58 +1818,57 @@
       <c r="F11">
         <v>9</v>
       </c>
-      <c r="G11" t="str">
-        <f t="shared" si="3"/>
-        <v>AK9</v>
+      <c r="G11">
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
       <c r="K11">
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M11">
+        <f t="shared" si="6"/>
+        <v>10011</v>
+      </c>
+      <c r="N11" t="s">
+        <v>125</v>
+      </c>
+      <c r="O11" t="s">
+        <v>112</v>
+      </c>
+      <c r="P11" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>117</v>
+      </c>
+      <c r="R11" t="str">
         <f t="shared" si="7"/>
-        <v>10011</v>
-      </c>
-      <c r="N11" t="s">
-        <v>127</v>
-      </c>
-      <c r="O11" t="s">
-        <v>114</v>
-      </c>
-      <c r="P11" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>119</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" si="8"/>
         <v>088728372780</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>endang@gmail.com</v>
       </c>
       <c r="Z11">
         <v>9</v>
       </c>
       <c r="AA11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AB11" s="1">
+        <f t="shared" si="8"/>
+        <v>0.53125</v>
+      </c>
+      <c r="AC11" s="1">
         <f t="shared" si="9"/>
-        <v>0.53125</v>
-      </c>
-      <c r="AC11" s="1">
-        <f t="shared" si="10"/>
         <v>0.5625</v>
       </c>
       <c r="AD11" t="str">
@@ -1825,11 +1879,11 @@
         <v>7</v>
       </c>
       <c r="AN11" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>12:45 - 13:30</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1846,58 +1900,57 @@
       <c r="F12">
         <v>10</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" ref="G12:G75" si="12">I12&amp;(MID(G11,3,100)+1)</f>
-        <v>AK10</v>
+      <c r="G12">
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
       </c>
       <c r="K12">
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M12">
+        <f t="shared" si="6"/>
+        <v>10012</v>
+      </c>
+      <c r="N12" t="s">
+        <v>126</v>
+      </c>
+      <c r="O12" t="s">
+        <v>127</v>
+      </c>
+      <c r="P12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>117</v>
+      </c>
+      <c r="R12" t="str">
         <f t="shared" si="7"/>
-        <v>10012</v>
-      </c>
-      <c r="N12" t="s">
-        <v>128</v>
-      </c>
-      <c r="O12" t="s">
-        <v>129</v>
-      </c>
-      <c r="P12" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>119</v>
-      </c>
-      <c r="R12" t="str">
-        <f t="shared" si="8"/>
         <v>088728372781</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>maruf@gmail.com</v>
       </c>
       <c r="Z12">
         <v>10</v>
       </c>
       <c r="AA12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AB12" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AC12" s="1">
         <f t="shared" si="9"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AC12" s="1">
-        <f t="shared" si="10"/>
         <v>0.59375</v>
       </c>
       <c r="AD12" t="str">
@@ -1908,11 +1961,11 @@
         <v>8</v>
       </c>
       <c r="AN12" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>13:30 - 14:15</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1929,28 +1982,27 @@
       <c r="F13">
         <v>11</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="12"/>
-        <v>AK11</v>
+      <c r="G13">
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
       <c r="Z13">
         <v>11</v>
       </c>
       <c r="AA13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB13" s="1">
+        <f t="shared" si="8"/>
+        <v>0.59375</v>
+      </c>
+      <c r="AC13" s="1">
         <f t="shared" si="9"/>
-        <v>0.59375</v>
-      </c>
-      <c r="AC13" s="1">
-        <f t="shared" si="10"/>
         <v>0.625</v>
       </c>
       <c r="AD13" t="str">
@@ -1961,11 +2013,11 @@
         <v>9</v>
       </c>
       <c r="AN13" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>14:15 - 15:00</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1982,1125 +2034,1050 @@
       <c r="F14">
         <v>12</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="12"/>
-        <v>AK12</v>
+      <c r="G14">
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41">
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>13</v>
       </c>
-      <c r="G15" t="str">
-        <f t="shared" si="12"/>
-        <v>AK13</v>
+      <c r="G15">
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:41">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>14</v>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" si="12"/>
-        <v>AK14</v>
+      <c r="G16">
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>15</v>
       </c>
-      <c r="G17" t="str">
-        <f t="shared" si="12"/>
-        <v>AK15</v>
+      <c r="G17">
+        <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="6:9">
+        <v>54</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>16</v>
       </c>
-      <c r="G18" t="str">
-        <f t="shared" si="12"/>
-        <v>AK16</v>
+      <c r="G18">
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="6:9">
+        <v>23</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>17</v>
       </c>
-      <c r="G19" t="str">
-        <f t="shared" si="12"/>
-        <v>AK17</v>
+      <c r="G19">
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="6:9">
+        <v>24</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>18</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="12"/>
-        <v>AK18</v>
+      <c r="G20">
+        <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="6:9">
+        <v>25</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>19</v>
       </c>
-      <c r="G21" t="str">
-        <f t="shared" si="12"/>
-        <v>AK19</v>
+      <c r="G21">
+        <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="6:9">
+        <v>55</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="G22" t="str">
-        <f t="shared" si="12"/>
-        <v>AK20</v>
+      <c r="G22">
+        <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="6:9">
+        <v>26</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>21</v>
       </c>
-      <c r="G23" t="str">
-        <f t="shared" si="12"/>
-        <v>AK21</v>
+      <c r="G23">
+        <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="6:9">
+        <v>27</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>22</v>
       </c>
-      <c r="G24" t="str">
-        <f t="shared" si="12"/>
-        <v>AK22</v>
+      <c r="G24">
+        <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="6:9">
+        <v>28</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>23</v>
       </c>
-      <c r="G25" t="str">
-        <f t="shared" si="12"/>
-        <v>AK23</v>
+      <c r="G25">
+        <v>23</v>
       </c>
       <c r="H25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="6:9">
+        <v>29</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>24</v>
       </c>
-      <c r="G26" t="str">
-        <f>I26&amp;1</f>
-        <v>MM1</v>
+      <c r="G26">
+        <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="6:9">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>25</v>
       </c>
-      <c r="G27" t="str">
-        <f t="shared" si="12"/>
-        <v>MM2</v>
+      <c r="G27">
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="6:9">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>26</v>
       </c>
-      <c r="G28" t="str">
-        <f t="shared" si="12"/>
-        <v>MM3</v>
+      <c r="G28">
+        <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="6:9">
+        <v>11</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29">
         <v>27</v>
       </c>
-      <c r="G29" t="str">
-        <f t="shared" si="12"/>
-        <v>MM4</v>
+      <c r="G29">
+        <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="6:9">
+        <v>12</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F30">
         <v>28</v>
       </c>
-      <c r="G30" t="str">
-        <f t="shared" si="12"/>
-        <v>MM5</v>
+      <c r="G30">
+        <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="6:9">
+        <v>13</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F31">
         <v>29</v>
       </c>
-      <c r="G31" t="str">
-        <f t="shared" si="12"/>
-        <v>MM6</v>
+      <c r="G31">
+        <v>29</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="6:9">
+        <v>14</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F32">
         <v>30</v>
       </c>
-      <c r="G32" t="str">
-        <f t="shared" si="12"/>
-        <v>MM7</v>
+      <c r="G32">
+        <v>30</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9">
+        <v>15</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>31</v>
       </c>
-      <c r="G33" t="str">
-        <f t="shared" si="12"/>
-        <v>MM8</v>
+      <c r="G33">
+        <v>31</v>
       </c>
       <c r="H33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>32</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" si="12"/>
-        <v>MM9</v>
+      <c r="G34">
+        <v>32</v>
       </c>
       <c r="H34" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9">
+        <v>17</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>33</v>
       </c>
-      <c r="G35" t="str">
-        <f t="shared" si="12"/>
-        <v>MM10</v>
+      <c r="G35">
+        <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="6:9">
+        <v>18</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>34</v>
       </c>
-      <c r="G36" t="str">
-        <f t="shared" si="12"/>
-        <v>MM11</v>
+      <c r="G36">
+        <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="6:9">
+        <v>31</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>35</v>
       </c>
-      <c r="G37" t="str">
-        <f t="shared" si="12"/>
-        <v>MM12</v>
+      <c r="G37">
+        <v>35</v>
       </c>
       <c r="H37" t="s">
-        <v>32</v>
-      </c>
-      <c r="I37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="6:9">
+        <v>30</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>36</v>
       </c>
-      <c r="G38" t="str">
-        <f t="shared" si="12"/>
-        <v>MM13</v>
+      <c r="G38">
+        <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="6:9">
+        <v>32</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>37</v>
       </c>
-      <c r="G39" t="str">
-        <f t="shared" si="12"/>
-        <v>MM14</v>
+      <c r="G39">
+        <v>37</v>
       </c>
       <c r="H39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="6:9">
+        <v>33</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>38</v>
       </c>
-      <c r="G40" t="str">
-        <f t="shared" si="12"/>
-        <v>MM15</v>
+      <c r="G40">
+        <v>38</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="6:9">
+        <v>34</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>39</v>
       </c>
-      <c r="G41" t="str">
-        <f t="shared" si="12"/>
-        <v>MM16</v>
+      <c r="G41">
+        <v>39</v>
       </c>
       <c r="H41" t="s">
-        <v>37</v>
-      </c>
-      <c r="I41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="6:9">
+        <v>35</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>40</v>
       </c>
-      <c r="G42" t="str">
-        <f t="shared" si="12"/>
-        <v>MM17</v>
+      <c r="G42">
+        <v>40</v>
       </c>
       <c r="H42" t="s">
-        <v>38</v>
-      </c>
-      <c r="I42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="6:9">
+        <v>36</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43">
         <v>41</v>
       </c>
-      <c r="G43" t="str">
-        <f t="shared" si="12"/>
-        <v>MM18</v>
+      <c r="G43">
+        <v>41</v>
       </c>
       <c r="H43" t="s">
-        <v>39</v>
-      </c>
-      <c r="I43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="6:9">
+        <v>37</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44">
         <v>42</v>
       </c>
-      <c r="G44" t="str">
-        <f t="shared" si="12"/>
-        <v>MM19</v>
+      <c r="G44">
+        <v>42</v>
       </c>
       <c r="H44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="6:9">
+        <v>38</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45">
         <v>43</v>
       </c>
-      <c r="G45" t="str">
-        <f t="shared" si="12"/>
-        <v>MM20</v>
+      <c r="G45">
+        <v>43</v>
       </c>
       <c r="H45" t="s">
-        <v>41</v>
-      </c>
-      <c r="I45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="6:9">
+        <v>39</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>44</v>
       </c>
-      <c r="G46" t="str">
-        <f t="shared" si="12"/>
-        <v>MM21</v>
+      <c r="G46">
+        <v>44</v>
       </c>
       <c r="H46" t="s">
-        <v>31</v>
-      </c>
-      <c r="I46" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="6:9">
+        <v>29</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>45</v>
       </c>
-      <c r="G47" t="str">
-        <f>I47&amp;1</f>
-        <v>AP1</v>
+      <c r="G47">
+        <v>45</v>
       </c>
       <c r="H47" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="6:9">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>46</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" si="12"/>
-        <v>AP2</v>
+      <c r="G48">
+        <v>46</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
-      </c>
-      <c r="I48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="6:9">
+        <v>9</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49">
         <v>47</v>
       </c>
-      <c r="G49" t="str">
-        <f t="shared" si="12"/>
-        <v>AP3</v>
+      <c r="G49">
+        <v>47</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="6:9">
+        <v>11</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F50">
         <v>48</v>
       </c>
-      <c r="G50" t="str">
-        <f t="shared" si="12"/>
-        <v>AP4</v>
+      <c r="G50">
+        <v>48</v>
       </c>
       <c r="H50" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="6:9">
+        <v>12</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F51">
         <v>49</v>
       </c>
-      <c r="G51" t="str">
-        <f t="shared" si="12"/>
-        <v>AP5</v>
+      <c r="G51">
+        <v>49</v>
       </c>
       <c r="H51" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="6:9">
+        <v>13</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F52">
         <v>50</v>
       </c>
-      <c r="G52" t="str">
-        <f t="shared" si="12"/>
-        <v>AP6</v>
+      <c r="G52">
+        <v>50</v>
       </c>
       <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="6:9">
+        <v>14</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>51</v>
       </c>
-      <c r="G53" t="str">
-        <f t="shared" si="12"/>
-        <v>AP7</v>
+      <c r="G53">
+        <v>51</v>
       </c>
       <c r="H53" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="6:9">
+        <v>15</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>52</v>
       </c>
-      <c r="G54" t="str">
-        <f t="shared" si="12"/>
-        <v>AP8</v>
+      <c r="G54">
+        <v>52</v>
       </c>
       <c r="H54" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="6:9">
+        <v>16</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>53</v>
       </c>
-      <c r="G55" t="str">
-        <f t="shared" si="12"/>
-        <v>AP9</v>
+      <c r="G55">
+        <v>53</v>
       </c>
       <c r="H55" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="6:9">
+        <v>17</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>54</v>
       </c>
-      <c r="G56" t="str">
-        <f t="shared" si="12"/>
-        <v>AP10</v>
+      <c r="G56">
+        <v>54</v>
       </c>
       <c r="H56" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="6:9">
+        <v>18</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>55</v>
       </c>
-      <c r="G57" t="str">
-        <f t="shared" si="12"/>
-        <v>AP11</v>
+      <c r="G57">
+        <v>55</v>
       </c>
       <c r="H57" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="6:9">
+        <v>19</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>56</v>
       </c>
-      <c r="G58" t="str">
-        <f t="shared" si="12"/>
-        <v>AP12</v>
+      <c r="G58">
+        <v>56</v>
       </c>
       <c r="H58" t="s">
-        <v>22</v>
-      </c>
-      <c r="I58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="6:9">
+        <v>20</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>57</v>
       </c>
-      <c r="G59" t="str">
-        <f t="shared" si="12"/>
-        <v>AP13</v>
+      <c r="G59">
+        <v>57</v>
       </c>
       <c r="H59" t="s">
-        <v>23</v>
-      </c>
-      <c r="I59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="6:9">
+        <v>21</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F60">
         <v>58</v>
       </c>
-      <c r="G60" t="str">
-        <f t="shared" si="12"/>
-        <v>AP14</v>
+      <c r="G60">
+        <v>58</v>
       </c>
       <c r="H60" t="s">
-        <v>42</v>
-      </c>
-      <c r="I60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="6:9">
+        <v>40</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F61">
         <v>59</v>
       </c>
-      <c r="G61" t="str">
-        <f t="shared" si="12"/>
-        <v>AP15</v>
+      <c r="G61">
+        <v>59</v>
       </c>
       <c r="H61" t="s">
-        <v>44</v>
-      </c>
-      <c r="I61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="6:9">
+        <v>42</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F62">
         <v>60</v>
       </c>
-      <c r="G62" t="str">
-        <f t="shared" si="12"/>
-        <v>AP16</v>
+      <c r="G62">
+        <v>60</v>
       </c>
       <c r="H62" t="s">
-        <v>45</v>
-      </c>
-      <c r="I62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="6:9">
+        <v>43</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F63">
         <v>61</v>
       </c>
-      <c r="G63" t="str">
-        <f t="shared" si="12"/>
-        <v>AP17</v>
+      <c r="G63">
+        <v>61</v>
       </c>
       <c r="H63" t="s">
-        <v>43</v>
-      </c>
-      <c r="I63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="6:9">
+        <v>41</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F64">
         <v>62</v>
       </c>
-      <c r="G64" t="str">
-        <f t="shared" si="12"/>
-        <v>AP18</v>
+      <c r="G64">
+        <v>62</v>
       </c>
       <c r="H64" t="s">
-        <v>46</v>
-      </c>
-      <c r="I64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="6:9">
+        <v>44</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F65">
         <v>63</v>
       </c>
-      <c r="G65" t="str">
-        <f t="shared" si="12"/>
-        <v>AP19</v>
+      <c r="G65">
+        <v>63</v>
       </c>
       <c r="H65" t="s">
-        <v>47</v>
-      </c>
-      <c r="I65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="6:9">
+        <v>45</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F66">
         <v>64</v>
       </c>
-      <c r="G66" t="str">
-        <f t="shared" si="12"/>
-        <v>AP20</v>
+      <c r="G66">
+        <v>64</v>
       </c>
       <c r="H66" t="s">
-        <v>48</v>
-      </c>
-      <c r="I66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="6:9">
+        <v>46</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F67">
         <v>65</v>
       </c>
-      <c r="G67" t="str">
-        <f t="shared" si="12"/>
-        <v>AP21</v>
+      <c r="G67">
+        <v>65</v>
       </c>
       <c r="H67" t="s">
-        <v>31</v>
-      </c>
-      <c r="I67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="6:9">
+        <v>29</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F68">
         <v>66</v>
       </c>
-      <c r="G68" t="str">
-        <f>I68&amp;1</f>
-        <v>PM1</v>
+      <c r="G68">
+        <v>66</v>
       </c>
       <c r="H68" t="s">
-        <v>12</v>
-      </c>
-      <c r="I68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="6:9">
+        <v>10</v>
+      </c>
+      <c r="I68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F69">
         <v>67</v>
       </c>
-      <c r="G69" t="str">
-        <f t="shared" si="12"/>
-        <v>PM2</v>
+      <c r="G69">
+        <v>67</v>
       </c>
       <c r="H69" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="6:9">
+        <v>9</v>
+      </c>
+      <c r="I69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F70">
         <v>68</v>
       </c>
-      <c r="G70" t="str">
-        <f t="shared" si="12"/>
-        <v>PM3</v>
+      <c r="G70">
+        <v>68</v>
       </c>
       <c r="H70" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="6:9">
+        <v>11</v>
+      </c>
+      <c r="I70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F71">
         <v>69</v>
       </c>
-      <c r="G71" t="str">
-        <f t="shared" si="12"/>
-        <v>PM4</v>
+      <c r="G71">
+        <v>69</v>
       </c>
       <c r="H71" t="s">
-        <v>14</v>
-      </c>
-      <c r="I71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="6:9">
+        <v>12</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F72">
         <v>70</v>
       </c>
-      <c r="G72" t="str">
-        <f t="shared" si="12"/>
-        <v>PM5</v>
+      <c r="G72">
+        <v>70</v>
       </c>
       <c r="H72" t="s">
-        <v>15</v>
-      </c>
-      <c r="I72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="6:9">
+        <v>13</v>
+      </c>
+      <c r="I72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F73">
         <v>71</v>
       </c>
-      <c r="G73" t="str">
-        <f t="shared" si="12"/>
-        <v>PM6</v>
+      <c r="G73">
+        <v>71</v>
       </c>
       <c r="H73" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="6:9">
+        <v>14</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F74">
         <v>72</v>
       </c>
-      <c r="G74" t="str">
-        <f t="shared" si="12"/>
-        <v>PM7</v>
+      <c r="G74">
+        <v>72</v>
       </c>
       <c r="H74" t="s">
-        <v>17</v>
-      </c>
-      <c r="I74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="6:9">
+        <v>15</v>
+      </c>
+      <c r="I74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F75">
         <v>73</v>
       </c>
-      <c r="G75" t="str">
-        <f t="shared" si="12"/>
-        <v>PM8</v>
+      <c r="G75">
+        <v>73</v>
       </c>
       <c r="H75" t="s">
-        <v>18</v>
-      </c>
-      <c r="I75" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="6:9">
+        <v>16</v>
+      </c>
+      <c r="I75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F76">
         <v>74</v>
       </c>
-      <c r="G76" t="str">
-        <f t="shared" ref="G76:G88" si="13">I76&amp;(MID(G75,3,100)+1)</f>
-        <v>PM9</v>
+      <c r="G76">
+        <v>74</v>
       </c>
       <c r="H76" t="s">
-        <v>19</v>
-      </c>
-      <c r="I76" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="6:9">
+        <v>17</v>
+      </c>
+      <c r="I76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F77">
         <v>75</v>
       </c>
-      <c r="G77" t="str">
-        <f t="shared" si="13"/>
-        <v>PM10</v>
+      <c r="G77">
+        <v>75</v>
       </c>
       <c r="H77" t="s">
-        <v>20</v>
-      </c>
-      <c r="I77" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="6:9">
+        <v>18</v>
+      </c>
+      <c r="I77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F78">
         <v>76</v>
       </c>
-      <c r="G78" t="str">
-        <f t="shared" si="13"/>
-        <v>PM11</v>
+      <c r="G78">
+        <v>76</v>
       </c>
       <c r="H78" t="s">
-        <v>21</v>
-      </c>
-      <c r="I78" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="6:9">
+        <v>19</v>
+      </c>
+      <c r="I78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F79">
         <v>77</v>
       </c>
-      <c r="G79" t="str">
-        <f t="shared" si="13"/>
-        <v>PM12</v>
+      <c r="G79">
+        <v>77</v>
       </c>
       <c r="H79" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="6:9">
+        <v>20</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F80">
         <v>78</v>
       </c>
-      <c r="G80" t="str">
-        <f t="shared" si="13"/>
-        <v>PM13</v>
+      <c r="G80">
+        <v>78</v>
       </c>
       <c r="H80" t="s">
-        <v>23</v>
-      </c>
-      <c r="I80" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="6:9">
+        <v>21</v>
+      </c>
+      <c r="I80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F81">
         <v>79</v>
       </c>
-      <c r="G81" t="str">
-        <f t="shared" si="13"/>
-        <v>PM14</v>
+      <c r="G81">
+        <v>79</v>
       </c>
       <c r="H81" t="s">
-        <v>49</v>
-      </c>
-      <c r="I81" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="6:9">
+        <v>47</v>
+      </c>
+      <c r="I81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F82">
         <v>80</v>
       </c>
-      <c r="G82" t="str">
-        <f t="shared" si="13"/>
-        <v>PM15</v>
+      <c r="G82">
+        <v>80</v>
       </c>
       <c r="H82" t="s">
-        <v>50</v>
-      </c>
-      <c r="I82" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="6:9">
+        <v>48</v>
+      </c>
+      <c r="I82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F83">
         <v>81</v>
       </c>
-      <c r="G83" t="str">
-        <f t="shared" si="13"/>
-        <v>PM16</v>
+      <c r="G83">
+        <v>81</v>
       </c>
       <c r="H83" t="s">
-        <v>51</v>
-      </c>
-      <c r="I83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="6:9">
+        <v>49</v>
+      </c>
+      <c r="I83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F84">
         <v>82</v>
       </c>
-      <c r="G84" t="str">
-        <f t="shared" si="13"/>
-        <v>PM17</v>
+      <c r="G84">
+        <v>82</v>
       </c>
       <c r="H84" t="s">
-        <v>52</v>
-      </c>
-      <c r="I84" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="6:9">
+        <v>50</v>
+      </c>
+      <c r="I84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F85">
         <v>83</v>
       </c>
-      <c r="G85" t="str">
-        <f t="shared" si="13"/>
-        <v>PM18</v>
+      <c r="G85">
+        <v>83</v>
       </c>
       <c r="H85" t="s">
-        <v>53</v>
-      </c>
-      <c r="I85" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="6:9">
+        <v>51</v>
+      </c>
+      <c r="I85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F86">
         <v>84</v>
       </c>
-      <c r="G86" t="str">
-        <f t="shared" si="13"/>
-        <v>PM19</v>
+      <c r="G86">
+        <v>84</v>
       </c>
       <c r="H86" t="s">
-        <v>54</v>
-      </c>
-      <c r="I86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="6:9">
+        <v>52</v>
+      </c>
+      <c r="I86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F87">
         <v>85</v>
       </c>
-      <c r="G87" t="str">
-        <f t="shared" si="13"/>
-        <v>PM20</v>
+      <c r="G87">
+        <v>85</v>
       </c>
       <c r="H87" t="s">
-        <v>55</v>
-      </c>
-      <c r="I87" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="6:9">
+        <v>53</v>
+      </c>
+      <c r="I87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F88">
         <v>86</v>
       </c>
-      <c r="G88" t="str">
-        <f t="shared" si="13"/>
-        <v>PM21</v>
+      <c r="G88">
+        <v>86</v>
       </c>
       <c r="H88" t="s">
-        <v>31</v>
-      </c>
-      <c r="I88" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="I88">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create data master (hari & sesi), data transaction (guru mata pelajaran)
</commit_message>
<xml_diff>
--- a/Rancangan Database Penjadwalan.xlsx
+++ b/Rancangan Database Penjadwalan.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25407"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github-repository\php-project\php-project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748F7C9A-DAFE-4BDB-8D6D-D07B62EA28D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
   <si>
     <t>Kelas</t>
   </si>
@@ -239,18 +233,9 @@
     <t>Tb_Sesi</t>
   </si>
   <si>
-    <t>Durasi</t>
-  </si>
-  <si>
     <t>Sesi</t>
   </si>
   <si>
-    <t>Jam_Mulai</t>
-  </si>
-  <si>
-    <t>Jam_Selesai</t>
-  </si>
-  <si>
     <t>Istirahat</t>
   </si>
   <si>
@@ -438,13 +423,25 @@
   </si>
   <si>
     <t>kategori_ mapel</t>
+  </si>
+  <si>
+    <t>kode_sesi</t>
+  </si>
+  <si>
+    <t>jam_mulai</t>
+  </si>
+  <si>
+    <t>jam_selesai</t>
+  </si>
+  <si>
+    <t>durasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,7 +540,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,27 +572,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -627,24 +606,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -820,42 +781,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="4" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="4" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="8.88671875" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="44" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="17" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="14.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="14.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="8.88671875" customWidth="1" outlineLevel="1"/>
     <col min="22" max="22" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="14.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="18.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="11.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="13.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="8.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="35" width="8.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="8.85546875" collapsed="1"/>
-    <col min="38" max="38" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="18.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="11.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="13.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="8.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="35" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -869,25 +829,37 @@
         <v>61</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Z1" t="s">
         <v>68</v>
       </c>
+      <c r="AC1" t="str">
+        <f>LOWER(AC2)</f>
+        <v>jam_mulai</v>
+      </c>
+      <c r="AD1" t="str">
+        <f>LOWER(AD2)</f>
+        <v>jam_selesai</v>
+      </c>
+      <c r="AE1" t="str">
+        <f>LOWER(AE2)</f>
+        <v>durasi</v>
+      </c>
       <c r="AF1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG1" t="s">
         <v>67</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="AK1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -904,13 +876,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -919,13 +891,13 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N2" t="s">
         <v>56</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="P2" t="s">
         <v>57</v>
@@ -943,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="V2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="W2" t="s">
         <v>62</v>
@@ -955,19 +927,19 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="AB2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AC2" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="AD2" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="AE2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AG2" t="s">
         <v>1</v>
@@ -982,19 +954,19 @@
         <v>1</v>
       </c>
       <c r="AL2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="AM2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AN2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AO2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1024,22 +996,22 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M3">
         <v>10003</v>
       </c>
       <c r="N3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" t="s">
         <v>112</v>
       </c>
-      <c r="P3" t="s">
-        <v>115</v>
-      </c>
       <c r="Q3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="R3" t="str">
         <f>"0"&amp;88728372772</f>
@@ -1057,45 +1029,45 @@
         <v>AK1g0010</v>
       </c>
       <c r="W3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB3" s="1">
+        <v>73</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
         <v>0.29166666666666669</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>0.32291666666666669</v>
       </c>
-      <c r="AD3" t="str">
-        <f t="shared" ref="AD3:AD13" si="1">HOUR(AC3-AB3)&amp;" Jam "&amp;MINUTE(AC3-AB3)&amp;" Menit"</f>
+      <c r="AE3" t="str">
+        <f t="shared" ref="AE3:AE13" si="1">HOUR(AD3-AC3)&amp;" Jam "&amp;MINUTE(AD3-AC3)&amp;" Menit"</f>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AE3">
-        <v>1</v>
-      </c>
       <c r="AG3">
         <v>1</v>
       </c>
       <c r="AH3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AI3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AN3" s="1" t="str">
-        <f>TEXT(AB3,"hh:mm")&amp;" - "&amp;TEXT(AC3,"hh:mm")</f>
+        <f>TEXT(AC3,"hh:mm")&amp;" - "&amp;TEXT(AD3,"hh:mm")</f>
         <v>07:00 - 07:45</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1125,23 +1097,23 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M4">
         <f>M3+1</f>
         <v>10004</v>
       </c>
       <c r="N4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="O4" t="s">
+        <v>111</v>
+      </c>
+      <c r="P4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q4" t="s">
         <v>114</v>
-      </c>
-      <c r="P4" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>117</v>
       </c>
       <c r="R4" t="str">
         <f>"0"&amp;R3+1</f>
@@ -1159,7 +1131,7 @@
         <v>2g0010</v>
       </c>
       <c r="W4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X4">
         <f t="shared" ref="X4:X10" si="4">G4</f>
@@ -1169,37 +1141,37 @@
         <v>2</v>
       </c>
       <c r="AA4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB4" s="1">
-        <f>AC3</f>
+        <v>74</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>AD3</f>
         <v>0.32291666666666669</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="1">
         <v>0.35416666666666669</v>
       </c>
-      <c r="AD4" t="str">
+      <c r="AE4" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AE4">
-        <v>2</v>
-      </c>
       <c r="AG4">
         <v>2</v>
       </c>
       <c r="AH4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AI4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AN4" s="1" t="str">
-        <f t="shared" ref="AN4:AN13" si="5">TEXT(AB4,"hh:mm")&amp;" - "&amp;TEXT(AC4,"hh:mm")</f>
+        <f t="shared" ref="AN4:AN13" si="5">TEXT(AC4,"hh:mm")&amp;" - "&amp;TEXT(AD4,"hh:mm")</f>
         <v>07:45 - 08:30</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1229,23 +1201,23 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:M12" si="6">M4+1</f>
         <v>10005</v>
       </c>
       <c r="N5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" ref="R5:R12" si="7">"0"&amp;R4+1</f>
@@ -1263,7 +1235,7 @@
         <v>3g0010</v>
       </c>
       <c r="W5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X5">
         <f t="shared" si="4"/>
@@ -1273,37 +1245,37 @@
         <v>3</v>
       </c>
       <c r="AA5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB5" s="1">
-        <f t="shared" ref="AB5:AB13" si="8">AC4</f>
+        <v>75</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" ref="AC5:AC13" si="8">AD4</f>
         <v>0.35416666666666669</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AD5" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AE5" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AE5">
-        <v>3</v>
-      </c>
       <c r="AG5">
         <v>3</v>
       </c>
       <c r="AH5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="AI5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AN5" s="1" t="str">
         <f t="shared" si="5"/>
         <v>08:30 - 09:15</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1333,23 +1305,23 @@
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M6">
         <f t="shared" si="6"/>
         <v>10006</v>
       </c>
       <c r="N6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="7"/>
@@ -1367,7 +1339,7 @@
         <v>4g0010</v>
       </c>
       <c r="W6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X6">
         <f t="shared" si="4"/>
@@ -1377,38 +1349,38 @@
         <v>4</v>
       </c>
       <c r="AA6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB6" s="1">
+        <v>71</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC6" s="1">
         <f t="shared" si="8"/>
         <v>0.38541666666666669</v>
       </c>
-      <c r="AC6" s="1">
-        <f>AB6+15/1440</f>
+      <c r="AD6" s="1">
+        <f>AC6+15/1440</f>
         <v>0.39583333333333337</v>
       </c>
-      <c r="AD6" t="str">
+      <c r="AE6" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 15 Menit</v>
       </c>
-      <c r="AE6" t="s">
-        <v>73</v>
-      </c>
       <c r="AG6">
         <v>4</v>
       </c>
       <c r="AH6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AI6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AN6" s="1" t="str">
         <f t="shared" si="5"/>
         <v>09:15 - 09:30</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1438,23 +1410,23 @@
         <v>5</v>
       </c>
       <c r="L7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M7">
         <f t="shared" si="6"/>
         <v>10007</v>
       </c>
       <c r="N7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="O7" t="s">
+        <v>109</v>
+      </c>
+      <c r="P7" t="s">
         <v>112</v>
       </c>
-      <c r="P7" t="s">
-        <v>115</v>
-      </c>
       <c r="Q7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="7"/>
@@ -1472,7 +1444,7 @@
         <v>5g0010</v>
       </c>
       <c r="W7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X7">
         <f t="shared" si="4"/>
@@ -1482,38 +1454,38 @@
         <v>5</v>
       </c>
       <c r="AA7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB7" s="1">
+        <v>76</v>
+      </c>
+      <c r="AB7">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="1">
         <f t="shared" si="8"/>
         <v>0.39583333333333337</v>
       </c>
-      <c r="AC7" s="1">
-        <f t="shared" ref="AC7:AC13" si="9">AB7+45/1440</f>
+      <c r="AD7" s="1">
+        <f t="shared" ref="AD7:AD13" si="9">AC7+45/1440</f>
         <v>0.42708333333333337</v>
       </c>
-      <c r="AD7" t="str">
+      <c r="AE7" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AE7">
-        <v>4</v>
-      </c>
       <c r="AG7">
         <v>5</v>
       </c>
       <c r="AH7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AI7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AN7" s="1" t="str">
         <f t="shared" si="5"/>
         <v>09:30 - 10:15</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1543,23 +1515,23 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M8">
         <f t="shared" si="6"/>
         <v>10008</v>
       </c>
       <c r="N8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="O8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="P8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="7"/>
@@ -1577,7 +1549,7 @@
         <v>6g0010</v>
       </c>
       <c r="W8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X8">
         <f t="shared" si="4"/>
@@ -1587,29 +1559,29 @@
         <v>6</v>
       </c>
       <c r="AA8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB8" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB8">
+        <v>5</v>
+      </c>
+      <c r="AC8" s="1">
         <f t="shared" si="8"/>
         <v>0.42708333333333337</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AD8" s="1">
         <f t="shared" si="9"/>
         <v>0.45833333333333337</v>
       </c>
-      <c r="AD8" t="str">
+      <c r="AE8" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
-      </c>
-      <c r="AE8">
-        <v>5</v>
       </c>
       <c r="AN8" s="1" t="str">
         <f t="shared" si="5"/>
         <v>10:15 - 11:00</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1639,23 +1611,23 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M9">
         <f t="shared" si="6"/>
         <v>10009</v>
       </c>
       <c r="N9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="P9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="7"/>
@@ -1673,7 +1645,7 @@
         <v>7g0010</v>
       </c>
       <c r="W9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X9">
         <f t="shared" si="4"/>
@@ -1683,29 +1655,29 @@
         <v>7</v>
       </c>
       <c r="AA9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB9" s="1">
+        <v>78</v>
+      </c>
+      <c r="AB9">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="1">
         <f t="shared" si="8"/>
         <v>0.45833333333333337</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AD9" s="1">
         <f t="shared" si="9"/>
         <v>0.48958333333333337</v>
       </c>
-      <c r="AD9" t="str">
+      <c r="AE9" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
-      </c>
-      <c r="AE9">
-        <v>6</v>
       </c>
       <c r="AN9" s="1" t="str">
         <f t="shared" si="5"/>
         <v>11:00 - 11:45</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1735,23 +1707,23 @@
         <v>8</v>
       </c>
       <c r="L10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M10">
         <f t="shared" si="6"/>
         <v>10010</v>
       </c>
       <c r="N10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" si="7"/>
@@ -1769,7 +1741,7 @@
         <v>8g0010</v>
       </c>
       <c r="W10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="X10">
         <f t="shared" si="4"/>
@@ -1779,29 +1751,29 @@
         <v>8</v>
       </c>
       <c r="AA10" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB10" s="1">
+        <v>72</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC10" s="1">
         <f t="shared" si="8"/>
         <v>0.48958333333333337</v>
       </c>
-      <c r="AC10" s="1">
-        <f>AB10+60/1440</f>
+      <c r="AD10" s="1">
+        <f>AC10+60/1440</f>
         <v>0.53125</v>
       </c>
-      <c r="AD10" t="str">
+      <c r="AE10" t="str">
         <f t="shared" si="1"/>
         <v>1 Jam 0 Menit</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>73</v>
       </c>
       <c r="AN10" s="1" t="str">
         <f t="shared" si="5"/>
         <v>11:45 - 12:45</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1831,23 +1803,23 @@
         <v>9</v>
       </c>
       <c r="L11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M11">
         <f t="shared" si="6"/>
         <v>10011</v>
       </c>
       <c r="N11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" t="s">
+        <v>109</v>
+      </c>
+      <c r="P11" t="s">
         <v>125</v>
       </c>
-      <c r="O11" t="s">
-        <v>112</v>
-      </c>
-      <c r="P11" t="s">
-        <v>128</v>
-      </c>
       <c r="Q11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="7"/>
@@ -1861,29 +1833,29 @@
         <v>9</v>
       </c>
       <c r="AA11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB11" s="1">
+        <v>79</v>
+      </c>
+      <c r="AB11">
+        <v>7</v>
+      </c>
+      <c r="AC11" s="1">
         <f t="shared" si="8"/>
         <v>0.53125</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AD11" s="1">
         <f t="shared" si="9"/>
         <v>0.5625</v>
       </c>
-      <c r="AD11" t="str">
+      <c r="AE11" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
-      </c>
-      <c r="AE11">
-        <v>7</v>
       </c>
       <c r="AN11" s="1" t="str">
         <f t="shared" si="5"/>
         <v>12:45 - 13:30</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1913,23 +1885,23 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M12">
         <f t="shared" si="6"/>
         <v>10012</v>
       </c>
       <c r="N12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Q12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="7"/>
@@ -1943,29 +1915,29 @@
         <v>10</v>
       </c>
       <c r="AA12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB12" s="1">
+        <v>80</v>
+      </c>
+      <c r="AB12">
+        <v>8</v>
+      </c>
+      <c r="AC12" s="1">
         <f t="shared" si="8"/>
         <v>0.5625</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AD12" s="1">
         <f t="shared" si="9"/>
         <v>0.59375</v>
       </c>
-      <c r="AD12" t="str">
+      <c r="AE12" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
-      </c>
-      <c r="AE12">
-        <v>8</v>
       </c>
       <c r="AN12" s="1" t="str">
         <f t="shared" si="5"/>
         <v>13:30 - 14:15</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1995,29 +1967,29 @@
         <v>11</v>
       </c>
       <c r="AA13" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB13" s="1">
+        <v>81</v>
+      </c>
+      <c r="AB13">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="1">
         <f t="shared" si="8"/>
         <v>0.59375</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AD13" s="1">
         <f t="shared" si="9"/>
         <v>0.625</v>
       </c>
-      <c r="AD13" t="str">
+      <c r="AE13" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
-      </c>
-      <c r="AE13">
-        <v>9</v>
       </c>
       <c r="AN13" s="1" t="str">
         <f t="shared" si="5"/>
         <v>14:15 - 15:00</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2044,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41">
       <c r="F15">
         <v>13</v>
       </c>
@@ -2058,7 +2030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41">
       <c r="F16">
         <v>14</v>
       </c>
@@ -2072,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:9">
       <c r="F17">
         <v>15</v>
       </c>
@@ -2086,7 +2058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:9">
       <c r="F18">
         <v>16</v>
       </c>
@@ -2100,7 +2072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:9">
       <c r="F19">
         <v>17</v>
       </c>
@@ -2114,7 +2086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:9">
       <c r="F20">
         <v>18</v>
       </c>
@@ -2128,7 +2100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:9">
       <c r="F21">
         <v>19</v>
       </c>
@@ -2142,7 +2114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:9">
       <c r="F22">
         <v>20</v>
       </c>
@@ -2156,7 +2128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:9">
       <c r="F23">
         <v>21</v>
       </c>
@@ -2170,7 +2142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:9">
       <c r="F24">
         <v>22</v>
       </c>
@@ -2184,7 +2156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:9">
       <c r="F25">
         <v>23</v>
       </c>
@@ -2198,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:9">
       <c r="F26">
         <v>24</v>
       </c>
@@ -2212,7 +2184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:9">
       <c r="F27">
         <v>25</v>
       </c>
@@ -2226,7 +2198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:9">
       <c r="F28">
         <v>26</v>
       </c>
@@ -2240,7 +2212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:9">
       <c r="F29">
         <v>27</v>
       </c>
@@ -2254,7 +2226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:9">
       <c r="F30">
         <v>28</v>
       </c>
@@ -2268,7 +2240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:9">
       <c r="F31">
         <v>29</v>
       </c>
@@ -2282,7 +2254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:9">
       <c r="F32">
         <v>30</v>
       </c>
@@ -2296,7 +2268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:9">
       <c r="F33">
         <v>31</v>
       </c>
@@ -2310,7 +2282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:9">
       <c r="F34">
         <v>32</v>
       </c>
@@ -2324,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:9">
       <c r="F35">
         <v>33</v>
       </c>
@@ -2338,7 +2310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:9">
       <c r="F36">
         <v>34</v>
       </c>
@@ -2352,7 +2324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:9">
       <c r="F37">
         <v>35</v>
       </c>
@@ -2366,7 +2338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:9">
       <c r="F38">
         <v>36</v>
       </c>
@@ -2380,7 +2352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:9">
       <c r="F39">
         <v>37</v>
       </c>
@@ -2394,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:9">
       <c r="F40">
         <v>38</v>
       </c>
@@ -2408,7 +2380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:9">
       <c r="F41">
         <v>39</v>
       </c>
@@ -2422,7 +2394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:9">
       <c r="F42">
         <v>40</v>
       </c>
@@ -2436,7 +2408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:9">
       <c r="F43">
         <v>41</v>
       </c>
@@ -2450,7 +2422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:9">
       <c r="F44">
         <v>42</v>
       </c>
@@ -2464,7 +2436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:9">
       <c r="F45">
         <v>43</v>
       </c>
@@ -2478,7 +2450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:9">
       <c r="F46">
         <v>44</v>
       </c>
@@ -2492,7 +2464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:9">
       <c r="F47">
         <v>45</v>
       </c>
@@ -2506,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:9">
       <c r="F48">
         <v>46</v>
       </c>
@@ -2520,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:9">
       <c r="F49">
         <v>47</v>
       </c>
@@ -2534,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:9">
       <c r="F50">
         <v>48</v>
       </c>
@@ -2548,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:9">
       <c r="F51">
         <v>49</v>
       </c>
@@ -2562,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:9">
       <c r="F52">
         <v>50</v>
       </c>
@@ -2576,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:9">
       <c r="F53">
         <v>51</v>
       </c>
@@ -2590,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:9">
       <c r="F54">
         <v>52</v>
       </c>
@@ -2604,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:9">
       <c r="F55">
         <v>53</v>
       </c>
@@ -2618,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:9">
       <c r="F56">
         <v>54</v>
       </c>
@@ -2632,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:9">
       <c r="F57">
         <v>55</v>
       </c>
@@ -2646,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:9">
       <c r="F58">
         <v>56</v>
       </c>
@@ -2660,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:9">
       <c r="F59">
         <v>57</v>
       </c>
@@ -2674,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:9">
       <c r="F60">
         <v>58</v>
       </c>
@@ -2688,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:9">
       <c r="F61">
         <v>59</v>
       </c>
@@ -2702,7 +2674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:9">
       <c r="F62">
         <v>60</v>
       </c>
@@ -2716,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:9">
       <c r="F63">
         <v>61</v>
       </c>
@@ -2730,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:9">
       <c r="F64">
         <v>62</v>
       </c>
@@ -2744,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:9">
       <c r="F65">
         <v>63</v>
       </c>
@@ -2758,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:9">
       <c r="F66">
         <v>64</v>
       </c>
@@ -2772,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:9">
       <c r="F67">
         <v>65</v>
       </c>
@@ -2786,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:9">
       <c r="F68">
         <v>66</v>
       </c>
@@ -2800,7 +2772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:9">
       <c r="F69">
         <v>67</v>
       </c>
@@ -2814,7 +2786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:9">
       <c r="F70">
         <v>68</v>
       </c>
@@ -2828,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:9">
       <c r="F71">
         <v>69</v>
       </c>
@@ -2842,7 +2814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:9">
       <c r="F72">
         <v>70</v>
       </c>
@@ -2856,7 +2828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:9">
       <c r="F73">
         <v>71</v>
       </c>
@@ -2870,7 +2842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:9">
       <c r="F74">
         <v>72</v>
       </c>
@@ -2884,7 +2856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:9">
       <c r="F75">
         <v>73</v>
       </c>
@@ -2898,7 +2870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:9">
       <c r="F76">
         <v>74</v>
       </c>
@@ -2912,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:9">
       <c r="F77">
         <v>75</v>
       </c>
@@ -2926,7 +2898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:9">
       <c r="F78">
         <v>76</v>
       </c>
@@ -2940,7 +2912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:9">
       <c r="F79">
         <v>77</v>
       </c>
@@ -2954,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:9">
       <c r="F80">
         <v>78</v>
       </c>
@@ -2968,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:9">
       <c r="F81">
         <v>79</v>
       </c>
@@ -2982,7 +2954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:9">
       <c r="F82">
         <v>80</v>
       </c>
@@ -2996,7 +2968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:9">
       <c r="F83">
         <v>81</v>
       </c>
@@ -3010,7 +2982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:9">
       <c r="F84">
         <v>82</v>
       </c>
@@ -3024,7 +2996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:9">
       <c r="F85">
         <v>83</v>
       </c>
@@ -3038,7 +3010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:9">
       <c r="F86">
         <v>84</v>
       </c>
@@ -3052,7 +3024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:9">
       <c r="F87">
         <v>85</v>
       </c>
@@ -3066,7 +3038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:9">
       <c r="F88">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
proccesing create data penjadwalan
</commit_message>
<xml_diff>
--- a/Rancangan Database Penjadwalan.xlsx
+++ b/Rancangan Database Penjadwalan.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25407"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github-repository\php-project\php-project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD97059A-04DB-4EC5-BAAF-4CFF8217A9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="139">
   <si>
     <t>Kelas</t>
   </si>
@@ -435,13 +441,19 @@
   </si>
   <si>
     <t>durasi</t>
+  </si>
+  <si>
+    <t>AP10</t>
+  </si>
+  <si>
+    <t>guru123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,7 +552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,9 +584,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,6 +636,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -781,41 +829,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AN5" sqref="AN5"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="7" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="4" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="8.85546875" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="44" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="17" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="8.85546875" customWidth="1" outlineLevel="1"/>
     <col min="22" max="22" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="14.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="18.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="11.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="9.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="13.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="8.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="35" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="18.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="11.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="13.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="8.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="35" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="21" customWidth="1"/>
+    <col min="39" max="39" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.5703125" customWidth="1"/>
+    <col min="41" max="41" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -859,7 +908,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -954,19 +1003,19 @@
         <v>1</v>
       </c>
       <c r="AL2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM2" t="s">
         <v>95</v>
       </c>
-      <c r="AM2" t="s">
-        <v>94</v>
-      </c>
       <c r="AN2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO2" t="s">
         <v>128</v>
       </c>
-      <c r="AO2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1062,12 +1111,23 @@
       <c r="AI3" t="s">
         <v>87</v>
       </c>
-      <c r="AN3" s="1" t="str">
-        <f>TEXT(AC3,"hh:mm")&amp;" - "&amp;TEXT(AD3,"hh:mm")</f>
-        <v>07:00 - 07:45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41">
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1166,12 +1226,23 @@
       <c r="AI4" t="s">
         <v>88</v>
       </c>
-      <c r="AN4" s="1" t="str">
-        <f t="shared" ref="AN4:AN13" si="5">TEXT(AC4,"hh:mm")&amp;" - "&amp;TEXT(AD4,"hh:mm")</f>
-        <v>07:45 - 08:30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
+      <c r="AK4">
+        <v>2</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1204,7 +1275,7 @@
         <v>100</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M12" si="6">M4+1</f>
+        <f t="shared" ref="M5:M12" si="5">M4+1</f>
         <v>10005</v>
       </c>
       <c r="N5" t="s">
@@ -1220,7 +1291,7 @@
         <v>113</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" ref="R5:R12" si="7">"0"&amp;R4+1</f>
+        <f t="shared" ref="R5:R12" si="6">"0"&amp;R4+1</f>
         <v>088728372774</v>
       </c>
       <c r="S5" t="str">
@@ -1251,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="AC5" s="1">
-        <f t="shared" ref="AC5:AC13" si="8">AD4</f>
+        <f t="shared" ref="AC5:AC13" si="7">AD4</f>
         <v>0.35416666666666669</v>
       </c>
       <c r="AD5" s="1">
@@ -1270,12 +1341,23 @@
       <c r="AI5" t="s">
         <v>89</v>
       </c>
-      <c r="AN5" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>08:30 - 09:15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
+      <c r="AK5">
+        <v>3</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1308,7 +1390,7 @@
         <v>101</v>
       </c>
       <c r="M6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10006</v>
       </c>
       <c r="N6" t="s">
@@ -1324,7 +1406,7 @@
         <v>114</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372775</v>
       </c>
       <c r="S6" t="str">
@@ -1355,7 +1437,7 @@
         <v>70</v>
       </c>
       <c r="AC6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.38541666666666669</v>
       </c>
       <c r="AD6" s="1">
@@ -1375,12 +1457,23 @@
       <c r="AI6" t="s">
         <v>90</v>
       </c>
-      <c r="AN6" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>09:15 - 09:30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41">
+      <c r="AK6">
+        <v>4</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1413,7 +1506,7 @@
         <v>102</v>
       </c>
       <c r="M7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10007</v>
       </c>
       <c r="N7" t="s">
@@ -1429,7 +1522,7 @@
         <v>113</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372776</v>
       </c>
       <c r="S7" t="str">
@@ -1460,11 +1553,11 @@
         <v>4</v>
       </c>
       <c r="AC7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.39583333333333337</v>
       </c>
       <c r="AD7" s="1">
-        <f t="shared" ref="AD7:AD13" si="9">AC7+45/1440</f>
+        <f t="shared" ref="AD7:AD13" si="8">AC7+45/1440</f>
         <v>0.42708333333333337</v>
       </c>
       <c r="AE7" t="str">
@@ -1480,12 +1573,23 @@
       <c r="AI7" t="s">
         <v>91</v>
       </c>
-      <c r="AN7" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>09:30 - 10:15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:41">
+      <c r="AK7">
+        <v>5</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1518,7 +1622,7 @@
         <v>103</v>
       </c>
       <c r="M8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10008</v>
       </c>
       <c r="N8" t="s">
@@ -1534,7 +1638,7 @@
         <v>114</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372777</v>
       </c>
       <c r="S8" t="str">
@@ -1565,23 +1669,34 @@
         <v>5</v>
       </c>
       <c r="AC8" s="1">
+        <f t="shared" si="7"/>
+        <v>0.42708333333333337</v>
+      </c>
+      <c r="AD8" s="1">
         <f t="shared" si="8"/>
-        <v>0.42708333333333337</v>
-      </c>
-      <c r="AD8" s="1">
-        <f t="shared" si="9"/>
         <v>0.45833333333333337</v>
       </c>
       <c r="AE8" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AN8" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>10:15 - 11:00</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41">
+      <c r="AK8">
+        <v>6</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1614,7 +1729,7 @@
         <v>104</v>
       </c>
       <c r="M9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10009</v>
       </c>
       <c r="N9" t="s">
@@ -1630,7 +1745,7 @@
         <v>114</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372778</v>
       </c>
       <c r="S9" t="str">
@@ -1661,23 +1776,34 @@
         <v>6</v>
       </c>
       <c r="AC9" s="1">
+        <f t="shared" si="7"/>
+        <v>0.45833333333333337</v>
+      </c>
+      <c r="AD9" s="1">
         <f t="shared" si="8"/>
-        <v>0.45833333333333337</v>
-      </c>
-      <c r="AD9" s="1">
-        <f t="shared" si="9"/>
         <v>0.48958333333333337</v>
       </c>
       <c r="AE9" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AN9" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>11:00 - 11:45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41">
+      <c r="AK9">
+        <v>7</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1710,7 +1836,7 @@
         <v>105</v>
       </c>
       <c r="M10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10010</v>
       </c>
       <c r="N10" t="s">
@@ -1726,11 +1852,11 @@
         <v>113</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372779</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" ref="S10:S12" si="10">LOWER(SUBSTITUTE(N10," ","."))&amp;"@gmail.com"</f>
+        <f t="shared" ref="S10:S12" si="9">LOWER(SUBSTITUTE(N10," ","."))&amp;"@gmail.com"</f>
         <v>ono.jaya@gmail.com</v>
       </c>
       <c r="U10">
@@ -1757,7 +1883,7 @@
         <v>70</v>
       </c>
       <c r="AC10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.48958333333333337</v>
       </c>
       <c r="AD10" s="1">
@@ -1768,12 +1894,23 @@
         <f t="shared" si="1"/>
         <v>1 Jam 0 Menit</v>
       </c>
-      <c r="AN10" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>11:45 - 12:45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41">
+      <c r="AK10">
+        <v>8</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1806,7 +1943,7 @@
         <v>106</v>
       </c>
       <c r="M11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10011</v>
       </c>
       <c r="N11" t="s">
@@ -1822,11 +1959,11 @@
         <v>114</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372780</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>endang@gmail.com</v>
       </c>
       <c r="Z11">
@@ -1839,23 +1976,34 @@
         <v>7</v>
       </c>
       <c r="AC11" s="1">
+        <f t="shared" si="7"/>
+        <v>0.53125</v>
+      </c>
+      <c r="AD11" s="1">
         <f t="shared" si="8"/>
-        <v>0.53125</v>
-      </c>
-      <c r="AD11" s="1">
-        <f t="shared" si="9"/>
         <v>0.5625</v>
       </c>
       <c r="AE11" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AN11" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>12:45 - 13:30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41">
+      <c r="AK11">
+        <v>9</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1888,7 +2036,7 @@
         <v>107</v>
       </c>
       <c r="M12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10012</v>
       </c>
       <c r="N12" t="s">
@@ -1904,11 +2052,11 @@
         <v>114</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>088728372781</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>maruf@gmail.com</v>
       </c>
       <c r="Z12">
@@ -1921,23 +2069,34 @@
         <v>8</v>
       </c>
       <c r="AC12" s="1">
+        <f t="shared" si="7"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AD12" s="1">
         <f t="shared" si="8"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AD12" s="1">
-        <f t="shared" si="9"/>
         <v>0.59375</v>
       </c>
       <c r="AE12" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AN12" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>13:30 - 14:15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41">
+      <c r="AK12">
+        <v>10</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1973,23 +2132,34 @@
         <v>9</v>
       </c>
       <c r="AC13" s="1">
+        <f t="shared" si="7"/>
+        <v>0.59375</v>
+      </c>
+      <c r="AD13" s="1">
         <f t="shared" si="8"/>
-        <v>0.59375</v>
-      </c>
-      <c r="AD13" s="1">
-        <f t="shared" si="9"/>
         <v>0.625</v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="1"/>
         <v>0 Jam 45 Menit</v>
       </c>
-      <c r="AN13" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>14:15 - 15:00</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41">
+      <c r="AK13">
+        <v>11</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2016,7 +2186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>13</v>
       </c>
@@ -2030,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>14</v>
       </c>
@@ -2044,7 +2214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="6:9">
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>15</v>
       </c>
@@ -2058,7 +2228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="6:9">
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>16</v>
       </c>
@@ -2072,7 +2242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="6:9">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>17</v>
       </c>
@@ -2086,7 +2256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="6:9">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>18</v>
       </c>
@@ -2100,7 +2270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="6:9">
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>19</v>
       </c>
@@ -2114,7 +2284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="6:9">
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>20</v>
       </c>
@@ -2128,7 +2298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="6:9">
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>21</v>
       </c>
@@ -2142,7 +2312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="6:9">
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>22</v>
       </c>
@@ -2156,7 +2326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="6:9">
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>23</v>
       </c>
@@ -2170,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="6:9">
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>24</v>
       </c>
@@ -2184,7 +2354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="6:9">
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>25</v>
       </c>
@@ -2198,7 +2368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="6:9">
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>26</v>
       </c>
@@ -2212,7 +2382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="6:9">
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29">
         <v>27</v>
       </c>
@@ -2226,7 +2396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="6:9">
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F30">
         <v>28</v>
       </c>
@@ -2240,7 +2410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="6:9">
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F31">
         <v>29</v>
       </c>
@@ -2254,7 +2424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="6:9">
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F32">
         <v>30</v>
       </c>
@@ -2268,7 +2438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="6:9">
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>31</v>
       </c>
@@ -2282,7 +2452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="6:9">
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>32</v>
       </c>
@@ -2296,7 +2466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="6:9">
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>33</v>
       </c>
@@ -2310,7 +2480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="6:9">
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>34</v>
       </c>
@@ -2324,7 +2494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="6:9">
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>35</v>
       </c>
@@ -2338,7 +2508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="6:9">
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>36</v>
       </c>
@@ -2352,7 +2522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="6:9">
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>37</v>
       </c>
@@ -2366,7 +2536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="6:9">
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>38</v>
       </c>
@@ -2380,7 +2550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="6:9">
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>39</v>
       </c>
@@ -2394,7 +2564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="6:9">
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>40</v>
       </c>
@@ -2408,7 +2578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="6:9">
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43">
         <v>41</v>
       </c>
@@ -2422,7 +2592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="6:9">
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44">
         <v>42</v>
       </c>
@@ -2436,7 +2606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="6:9">
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45">
         <v>43</v>
       </c>
@@ -2450,7 +2620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="6:9">
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>44</v>
       </c>
@@ -2464,7 +2634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="6:9">
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>45</v>
       </c>
@@ -2478,7 +2648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="6:9">
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>46</v>
       </c>
@@ -2492,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="6:9">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49">
         <v>47</v>
       </c>
@@ -2506,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="6:9">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F50">
         <v>48</v>
       </c>
@@ -2520,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="6:9">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F51">
         <v>49</v>
       </c>
@@ -2534,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="6:9">
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F52">
         <v>50</v>
       </c>
@@ -2548,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="6:9">
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>51</v>
       </c>
@@ -2562,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="6:9">
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>52</v>
       </c>
@@ -2576,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="6:9">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>53</v>
       </c>
@@ -2590,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="6:9">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>54</v>
       </c>
@@ -2604,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="6:9">
+    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>55</v>
       </c>
@@ -2618,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="6:9">
+    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>56</v>
       </c>
@@ -2632,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="6:9">
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>57</v>
       </c>
@@ -2646,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="6:9">
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F60">
         <v>58</v>
       </c>
@@ -2660,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="6:9">
+    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F61">
         <v>59</v>
       </c>
@@ -2674,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="6:9">
+    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F62">
         <v>60</v>
       </c>
@@ -2688,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="6:9">
+    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F63">
         <v>61</v>
       </c>
@@ -2702,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="6:9">
+    <row r="64" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F64">
         <v>62</v>
       </c>
@@ -2716,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="6:9">
+    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F65">
         <v>63</v>
       </c>
@@ -2730,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="6:9">
+    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F66">
         <v>64</v>
       </c>
@@ -2744,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="6:9">
+    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F67">
         <v>65</v>
       </c>
@@ -2758,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="6:9">
+    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F68">
         <v>66</v>
       </c>
@@ -2772,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="6:9">
+    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F69">
         <v>67</v>
       </c>
@@ -2786,7 +2956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="6:9">
+    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F70">
         <v>68</v>
       </c>
@@ -2800,7 +2970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="6:9">
+    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F71">
         <v>69</v>
       </c>
@@ -2814,7 +2984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="6:9">
+    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F72">
         <v>70</v>
       </c>
@@ -2828,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="6:9">
+    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F73">
         <v>71</v>
       </c>
@@ -2842,7 +3012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="6:9">
+    <row r="74" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F74">
         <v>72</v>
       </c>
@@ -2856,7 +3026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="6:9">
+    <row r="75" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F75">
         <v>73</v>
       </c>
@@ -2870,7 +3040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="6:9">
+    <row r="76" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F76">
         <v>74</v>
       </c>
@@ -2884,7 +3054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="6:9">
+    <row r="77" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F77">
         <v>75</v>
       </c>
@@ -2898,7 +3068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="6:9">
+    <row r="78" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F78">
         <v>76</v>
       </c>
@@ -2912,7 +3082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="6:9">
+    <row r="79" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F79">
         <v>77</v>
       </c>
@@ -2926,7 +3096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="6:9">
+    <row r="80" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F80">
         <v>78</v>
       </c>
@@ -2940,7 +3110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="6:9">
+    <row r="81" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F81">
         <v>79</v>
       </c>
@@ -2954,7 +3124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="6:9">
+    <row r="82" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F82">
         <v>80</v>
       </c>
@@ -2968,7 +3138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="6:9">
+    <row r="83" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F83">
         <v>81</v>
       </c>
@@ -2982,7 +3152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="6:9">
+    <row r="84" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F84">
         <v>82</v>
       </c>
@@ -2996,7 +3166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="6:9">
+    <row r="85" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F85">
         <v>83</v>
       </c>
@@ -3010,7 +3180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="6:9">
+    <row r="86" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F86">
         <v>84</v>
       </c>
@@ -3024,7 +3194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="6:9">
+    <row r="87" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F87">
         <v>85</v>
       </c>
@@ -3038,7 +3208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="6:9">
+    <row r="88" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F88">
         <v>86</v>
       </c>

</xml_diff>